<commit_message>
Some refactoring to prepare final manifest model
</commit_message>
<xml_diff>
--- a/ManifestTemplate.xlsx
+++ b/ManifestTemplate.xlsx
@@ -2113,7 +2113,7 @@
               <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
               <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
             </a:rPr>
-            <a:t>:  The abbreviated rank of the passenger.   For example:  SPC, SGT,  2LT, etc.   For civilians, this is a number representing their GS pay level.  For example:  7 for a GS-7, 10 for a GS-10, etc.</a:t>
+            <a:t>:  The abbreviated rank of the passenger.   For example:  SPC, SGT,  2LT, etc.   For civilians, this is a number representing their GS or WG pay level.  For example:  7 for a GS-7, 10 for a WG-10, etc.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -12258,7 +12258,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A36:M42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>

</xml_diff>